<commit_message>
Savepoint; FCRT 2.1.1-2 are complete and 100%; required nominal corrections including a 'state' nomen collision on TResponse; modified api post response route thru Request.Publish (~new) and not Request.Submit; determination made that Submit s/b restricted for internal app requests only while exposing the Publish function to the API was in fact cleaner; next up, FCRT 2.1.3-4 (3.Updates, 4.Leverages) ...
</commit_message>
<xml_diff>
--- a/~Documents/api-error.xlsx
+++ b/~Documents/api-error.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="150">
   <si>
     <t>Outcome Matrix</t>
   </si>
@@ -245,7 +245,10 @@
     <t>Unauthorized Instrument Position request from logged account</t>
   </si>
   <si>
-    <t>Invalid Order State</t>
+    <t>Invalid Order State metadata; unable to resolve state [${order.state}}] on Order: ${request}</t>
+  </si>
+  <si>
+    <t>Order not found for Request: ${request.clientOrderId || request.orderId}</t>
   </si>
   <si>
     <t>Pending</t>
@@ -475,10 +478,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -520,6 +523,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -528,24 +539,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,60 +571,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,9 +602,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -643,7 +624,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -651,9 +632,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -678,25 +681,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,7 +693,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,109 +705,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,7 +723,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,7 +813,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1566,11 +1569,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1586,41 +1613,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1657,9 +1649,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1668,152 +1671,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="62" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="59" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="59" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="61" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="59" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="62" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="56" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1993,9 +1996,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2391,17 +2391,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:M167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H151" sqref="H151"/>
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1"/>
   <cols>
     <col min="1" max="2" width="19.8666666666667" customWidth="1"/>
     <col min="3" max="7" width="14.5407407407407" style="3" customWidth="1"/>
-    <col min="8" max="8" width="68.3703703703704" style="3" customWidth="1"/>
+    <col min="8" max="8" width="93.1185185185185" style="3" customWidth="1"/>
     <col min="9" max="11" width="14.5407407407407" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2486,7 +2486,7 @@
       <c r="J5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2507,13 +2507,13 @@
       <c r="H6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="61">
+      <c r="I6" s="60">
         <v>0</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="K6" s="61" t="s">
         <v>17</v>
       </c>
       <c r="M6">
@@ -2534,13 +2534,13 @@
       <c r="H7" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="63">
+      <c r="I7" s="62">
         <v>312</v>
       </c>
-      <c r="J7" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="64"/>
+      <c r="J7" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" customFormat="1" spans="1:11">
       <c r="A8" s="10"/>
@@ -2555,13 +2555,13 @@
       <c r="H8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="63">
+      <c r="I8" s="62">
         <v>315</v>
       </c>
-      <c r="J8" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="64"/>
+      <c r="J8" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="63"/>
     </row>
     <row r="9" customFormat="1" spans="1:11">
       <c r="A9" s="10"/>
@@ -2576,13 +2576,13 @@
       <c r="H9" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="65" t="s">
+      <c r="I9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="66"/>
+      <c r="J9" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="65"/>
     </row>
     <row r="10" customFormat="1" spans="1:11">
       <c r="A10" s="10"/>
@@ -2605,7 +2605,7 @@
       <c r="J10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="63" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2628,7 +2628,7 @@
       <c r="J11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="64"/>
+      <c r="K11" s="63"/>
     </row>
     <row r="12" customFormat="1" spans="1:11">
       <c r="A12" s="10"/>
@@ -2649,7 +2649,7 @@
       <c r="J12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="64"/>
+      <c r="K12" s="63"/>
     </row>
     <row r="13" customFormat="1" spans="1:11">
       <c r="A13" s="10"/>
@@ -2664,13 +2664,13 @@
       <c r="H13" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="67" t="s">
+      <c r="I13" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="68"/>
+      <c r="J13" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="67"/>
     </row>
     <row r="14" customFormat="1" spans="1:11">
       <c r="A14" s="10"/>
@@ -2687,13 +2687,13 @@
       <c r="H14" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="69">
+      <c r="I14" s="68">
         <v>0</v>
       </c>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="K14" s="69" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2710,13 +2710,13 @@
       <c r="H15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="63">
-        <v>200</v>
-      </c>
-      <c r="J15" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="64"/>
+      <c r="I15" s="62">
+        <v>200</v>
+      </c>
+      <c r="J15" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="63"/>
     </row>
     <row r="16" customFormat="1" spans="1:11">
       <c r="A16" s="10"/>
@@ -2731,13 +2731,13 @@
       <c r="H16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="63">
+      <c r="I16" s="62">
         <v>315</v>
       </c>
-      <c r="J16" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="64"/>
+      <c r="J16" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="63"/>
     </row>
     <row r="17" customFormat="1" spans="1:11">
       <c r="A17" s="10"/>
@@ -2758,7 +2758,7 @@
       <c r="J17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="64"/>
+      <c r="K17" s="63"/>
     </row>
     <row r="18" customFormat="1" spans="1:11">
       <c r="A18" s="10"/>
@@ -2779,7 +2779,7 @@
       <c r="J18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="64"/>
+      <c r="K18" s="63"/>
     </row>
     <row r="19" customFormat="1" ht="14.85" spans="1:11">
       <c r="A19" s="21"/>
@@ -2794,13 +2794,13 @@
       <c r="H19" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="72"/>
+      <c r="J19" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="71"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="25" t="s">
@@ -2817,13 +2817,13 @@
         <v>14</v>
       </c>
       <c r="H20" s="57"/>
-      <c r="I20" s="73">
+      <c r="I20" s="72">
         <v>0</v>
       </c>
-      <c r="J20" s="73" t="s">
+      <c r="J20" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="64" t="s">
+      <c r="K20" s="63" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2838,13 +2838,13 @@
         <v>18</v>
       </c>
       <c r="H21" s="44"/>
-      <c r="I21" s="63">
+      <c r="I21" s="62">
         <v>201</v>
       </c>
-      <c r="J21" s="63" t="s">
+      <c r="J21" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="64"/>
+      <c r="K21" s="63"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="28"/>
@@ -2857,13 +2857,13 @@
         <v>17</v>
       </c>
       <c r="H22" s="44"/>
-      <c r="I22" s="63" t="s">
+      <c r="I22" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="64"/>
+      <c r="J22" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="63"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="28"/>
@@ -2884,7 +2884,7 @@
       <c r="J23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="64"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="28"/>
@@ -2903,7 +2903,7 @@
       <c r="J24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="64"/>
+      <c r="K24" s="63"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="29"/>
@@ -2922,7 +2922,7 @@
       <c r="J25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="64"/>
+      <c r="K25" s="63"/>
     </row>
     <row r="26" ht="14.85" spans="1:11">
       <c r="A26" s="31"/>
@@ -2935,13 +2935,13 @@
         <v>17</v>
       </c>
       <c r="H26" s="54"/>
-      <c r="I26" s="71" t="s">
+      <c r="I26" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="72"/>
+      <c r="J26" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="71"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="32" t="s">
@@ -2958,13 +2958,13 @@
         <v>14</v>
       </c>
       <c r="H27" s="41"/>
-      <c r="I27" s="61">
+      <c r="I27" s="60">
         <v>0</v>
       </c>
-      <c r="J27" s="61" t="s">
+      <c r="J27" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="62" t="s">
+      <c r="K27" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2979,13 +2979,13 @@
         <v>18</v>
       </c>
       <c r="H28" s="44"/>
-      <c r="I28" s="63">
+      <c r="I28" s="62">
         <v>201</v>
       </c>
-      <c r="J28" s="63" t="s">
+      <c r="J28" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K28" s="64"/>
+      <c r="K28" s="63"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="28"/>
@@ -2998,13 +2998,13 @@
         <v>17</v>
       </c>
       <c r="H29" s="44"/>
-      <c r="I29" s="63" t="s">
+      <c r="I29" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="64"/>
+      <c r="J29" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="63"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="28"/>
@@ -3025,7 +3025,7 @@
       <c r="J30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="64"/>
+      <c r="K30" s="63"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="28"/>
@@ -3044,7 +3044,7 @@
       <c r="J31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="64"/>
+      <c r="K31" s="63"/>
     </row>
     <row r="32" ht="14.85" spans="1:11">
       <c r="A32" s="31"/>
@@ -3057,13 +3057,13 @@
         <v>17</v>
       </c>
       <c r="H32" s="54"/>
-      <c r="I32" s="71" t="s">
+      <c r="I32" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="72"/>
+      <c r="J32" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="71"/>
     </row>
     <row r="33" customFormat="1" spans="1:11">
       <c r="A33" s="32" t="s">
@@ -3080,13 +3080,13 @@
         <v>14</v>
       </c>
       <c r="H33" s="41"/>
-      <c r="I33" s="61">
+      <c r="I33" s="60">
         <v>0</v>
       </c>
-      <c r="J33" s="61" t="s">
+      <c r="J33" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K33" s="62" t="s">
+      <c r="K33" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3101,13 +3101,13 @@
         <v>18</v>
       </c>
       <c r="H34" s="44"/>
-      <c r="I34" s="63">
+      <c r="I34" s="62">
         <v>201</v>
       </c>
-      <c r="J34" s="63" t="s">
+      <c r="J34" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="64"/>
+      <c r="K34" s="63"/>
     </row>
     <row r="35" customFormat="1" spans="1:11">
       <c r="A35" s="28"/>
@@ -3120,13 +3120,13 @@
         <v>17</v>
       </c>
       <c r="H35" s="44"/>
-      <c r="I35" s="63" t="s">
+      <c r="I35" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="64"/>
+      <c r="J35" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="63"/>
     </row>
     <row r="36" customFormat="1" spans="1:11">
       <c r="A36" s="28"/>
@@ -3147,7 +3147,7 @@
       <c r="J36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K36" s="64"/>
+      <c r="K36" s="63"/>
     </row>
     <row r="37" customFormat="1" spans="1:11">
       <c r="A37" s="28"/>
@@ -3166,7 +3166,7 @@
       <c r="J37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K37" s="64"/>
+      <c r="K37" s="63"/>
     </row>
     <row r="38" customFormat="1" ht="14.85" spans="1:11">
       <c r="A38" s="31"/>
@@ -3179,13 +3179,13 @@
         <v>17</v>
       </c>
       <c r="H38" s="54"/>
-      <c r="I38" s="71" t="s">
+      <c r="I38" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J38" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="72"/>
+      <c r="J38" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="71"/>
     </row>
     <row r="39" customFormat="1" spans="1:11">
       <c r="A39" s="32" t="s">
@@ -3204,13 +3204,13 @@
       <c r="H39" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I39" s="69">
+      <c r="I39" s="68">
         <v>0</v>
       </c>
-      <c r="J39" s="69" t="s">
+      <c r="J39" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="K39" s="70" t="s">
+      <c r="K39" s="69" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3227,13 +3227,13 @@
       <c r="H40" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="63">
-        <v>200</v>
-      </c>
-      <c r="J40" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="64"/>
+      <c r="I40" s="62">
+        <v>200</v>
+      </c>
+      <c r="J40" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="63"/>
     </row>
     <row r="41" customFormat="1" spans="1:11">
       <c r="A41" s="28"/>
@@ -3254,7 +3254,7 @@
       <c r="J41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K41" s="64"/>
+      <c r="K41" s="63"/>
     </row>
     <row r="42" customFormat="1" spans="1:11">
       <c r="A42" s="28"/>
@@ -3275,7 +3275,7 @@
       <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="64"/>
+      <c r="K42" s="63"/>
     </row>
     <row r="43" customFormat="1" ht="14.85" spans="1:11">
       <c r="A43" s="31"/>
@@ -3290,13 +3290,13 @@
       <c r="H43" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="I43" s="71" t="s">
+      <c r="I43" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="72"/>
+      <c r="J43" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="71"/>
     </row>
     <row r="44" customFormat="1" spans="1:11">
       <c r="A44" s="33" t="s">
@@ -3315,13 +3315,13 @@
       <c r="H44" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="I44" s="63">
+      <c r="I44" s="62">
         <v>410</v>
       </c>
-      <c r="J44" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="62" t="s">
+      <c r="J44" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3336,13 +3336,13 @@
         <v>14</v>
       </c>
       <c r="H45" s="44"/>
-      <c r="I45" s="63">
+      <c r="I45" s="62">
         <v>0</v>
       </c>
-      <c r="J45" s="63" t="s">
+      <c r="J45" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K45" s="64"/>
+      <c r="K45" s="63"/>
     </row>
     <row r="46" customFormat="1" spans="1:11">
       <c r="A46" s="28"/>
@@ -3355,13 +3355,13 @@
         <v>18</v>
       </c>
       <c r="H46" s="44"/>
-      <c r="I46" s="63">
+      <c r="I46" s="62">
         <v>201</v>
       </c>
-      <c r="J46" s="63" t="s">
+      <c r="J46" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="64"/>
+      <c r="K46" s="63"/>
     </row>
     <row r="47" customFormat="1" spans="1:11">
       <c r="A47" s="28"/>
@@ -3374,13 +3374,13 @@
         <v>17</v>
       </c>
       <c r="H47" s="44"/>
-      <c r="I47" s="63" t="s">
+      <c r="I47" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J47" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="64"/>
+      <c r="J47" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="63"/>
     </row>
     <row r="48" customFormat="1" spans="1:11">
       <c r="A48" s="28"/>
@@ -3399,7 +3399,7 @@
       <c r="J48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K48" s="64"/>
+      <c r="K48" s="63"/>
     </row>
     <row r="49" customFormat="1" spans="1:11">
       <c r="A49" s="28"/>
@@ -3418,7 +3418,7 @@
       <c r="J49" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="64"/>
+      <c r="K49" s="63"/>
     </row>
     <row r="50" customFormat="1" ht="14.85" spans="1:11">
       <c r="A50" s="31"/>
@@ -3431,13 +3431,13 @@
         <v>17</v>
       </c>
       <c r="H50" s="54"/>
-      <c r="I50" s="71" t="s">
+      <c r="I50" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K50" s="72"/>
+      <c r="J50" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="71"/>
     </row>
     <row r="51" customFormat="1" spans="1:11">
       <c r="A51" s="33" t="s">
@@ -3454,13 +3454,13 @@
         <v>45</v>
       </c>
       <c r="H51" s="44"/>
-      <c r="I51" s="63">
+      <c r="I51" s="62">
         <v>411</v>
       </c>
-      <c r="J51" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51" s="62" t="s">
+      <c r="J51" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3475,13 +3475,13 @@
         <v>14</v>
       </c>
       <c r="H52" s="44"/>
-      <c r="I52" s="63">
+      <c r="I52" s="62">
         <v>0</v>
       </c>
-      <c r="J52" s="63" t="s">
+      <c r="J52" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K52" s="64"/>
+      <c r="K52" s="63"/>
     </row>
     <row r="53" customFormat="1" spans="1:11">
       <c r="A53" s="28"/>
@@ -3494,13 +3494,13 @@
         <v>18</v>
       </c>
       <c r="H53" s="44"/>
-      <c r="I53" s="63">
+      <c r="I53" s="62">
         <v>201</v>
       </c>
-      <c r="J53" s="63" t="s">
+      <c r="J53" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K53" s="64"/>
+      <c r="K53" s="63"/>
     </row>
     <row r="54" customFormat="1" spans="1:11">
       <c r="A54" s="28"/>
@@ -3513,13 +3513,13 @@
         <v>17</v>
       </c>
       <c r="H54" s="44"/>
-      <c r="I54" s="63" t="s">
+      <c r="I54" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J54" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="64"/>
+      <c r="J54" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="63"/>
     </row>
     <row r="55" customFormat="1" spans="1:11">
       <c r="A55" s="28"/>
@@ -3538,7 +3538,7 @@
       <c r="J55" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K55" s="64"/>
+      <c r="K55" s="63"/>
     </row>
     <row r="56" customFormat="1" spans="1:11">
       <c r="A56" s="28"/>
@@ -3557,7 +3557,7 @@
       <c r="J56" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="64"/>
+      <c r="K56" s="63"/>
     </row>
     <row r="57" customFormat="1" ht="14.85" spans="1:11">
       <c r="A57" s="31"/>
@@ -3570,13 +3570,13 @@
         <v>17</v>
       </c>
       <c r="H57" s="54"/>
-      <c r="I57" s="71" t="s">
+      <c r="I57" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K57" s="72"/>
+      <c r="J57" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="71"/>
     </row>
     <row r="58" customFormat="1" spans="1:11">
       <c r="A58" s="32" t="s">
@@ -3593,13 +3593,13 @@
         <v>14</v>
       </c>
       <c r="H58" s="41"/>
-      <c r="I58" s="61">
+      <c r="I58" s="60">
         <v>0</v>
       </c>
-      <c r="J58" s="61" t="s">
+      <c r="J58" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K58" s="62" t="s">
+      <c r="K58" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3614,13 +3614,13 @@
         <v>18</v>
       </c>
       <c r="H59" s="44"/>
-      <c r="I59" s="63">
+      <c r="I59" s="62">
         <v>201</v>
       </c>
-      <c r="J59" s="63" t="s">
+      <c r="J59" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K59" s="64"/>
+      <c r="K59" s="63"/>
     </row>
     <row r="60" customFormat="1" spans="1:11">
       <c r="A60" s="28"/>
@@ -3633,13 +3633,13 @@
         <v>17</v>
       </c>
       <c r="H60" s="44"/>
-      <c r="I60" s="63" t="s">
+      <c r="I60" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J60" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K60" s="64"/>
+      <c r="J60" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="63"/>
     </row>
     <row r="61" customFormat="1" spans="1:11">
       <c r="A61" s="28"/>
@@ -3660,7 +3660,7 @@
       <c r="J61" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K61" s="64"/>
+      <c r="K61" s="63"/>
     </row>
     <row r="62" customFormat="1" spans="1:11">
       <c r="A62" s="28"/>
@@ -3679,7 +3679,7 @@
       <c r="J62" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K62" s="64"/>
+      <c r="K62" s="63"/>
     </row>
     <row r="63" customFormat="1" ht="14.85" spans="1:11">
       <c r="A63" s="31"/>
@@ -3692,13 +3692,13 @@
         <v>17</v>
       </c>
       <c r="H63" s="54"/>
-      <c r="I63" s="71" t="s">
+      <c r="I63" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J63" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" s="72"/>
+      <c r="J63" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K63" s="71"/>
     </row>
     <row r="64" customFormat="1" spans="1:11">
       <c r="A64" s="32" t="s">
@@ -3715,13 +3715,13 @@
         <v>14</v>
       </c>
       <c r="H64" s="41"/>
-      <c r="I64" s="61">
+      <c r="I64" s="60">
         <v>0</v>
       </c>
-      <c r="J64" s="61" t="s">
+      <c r="J64" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K64" s="62" t="s">
+      <c r="K64" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3736,13 +3736,13 @@
         <v>18</v>
       </c>
       <c r="H65" s="44"/>
-      <c r="I65" s="63">
+      <c r="I65" s="62">
         <v>201</v>
       </c>
-      <c r="J65" s="63" t="s">
+      <c r="J65" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K65" s="64"/>
+      <c r="K65" s="63"/>
     </row>
     <row r="66" customFormat="1" spans="1:11">
       <c r="A66" s="28"/>
@@ -3755,13 +3755,13 @@
         <v>17</v>
       </c>
       <c r="H66" s="44"/>
-      <c r="I66" s="63" t="s">
+      <c r="I66" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J66" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K66" s="64"/>
+      <c r="J66" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" s="63"/>
     </row>
     <row r="67" customFormat="1" spans="1:11">
       <c r="A67" s="28"/>
@@ -3782,7 +3782,7 @@
       <c r="J67" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K67" s="64"/>
+      <c r="K67" s="63"/>
     </row>
     <row r="68" customFormat="1" spans="1:11">
       <c r="A68" s="28"/>
@@ -3801,7 +3801,7 @@
       <c r="J68" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K68" s="64"/>
+      <c r="K68" s="63"/>
     </row>
     <row r="69" customFormat="1" ht="14.85" spans="1:11">
       <c r="A69" s="31"/>
@@ -3814,13 +3814,13 @@
         <v>17</v>
       </c>
       <c r="H69" s="54"/>
-      <c r="I69" s="71" t="s">
+      <c r="I69" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J69" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K69" s="72"/>
+      <c r="J69" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" s="71"/>
     </row>
     <row r="70" customFormat="1" spans="1:11">
       <c r="A70" s="35" t="s">
@@ -3839,13 +3839,13 @@
       <c r="H70" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I70" s="61">
+      <c r="I70" s="60">
         <v>415</v>
       </c>
-      <c r="J70" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="K70" s="62" t="s">
+      <c r="J70" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" s="61" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3860,13 +3860,13 @@
         <v>14</v>
       </c>
       <c r="H71" s="44"/>
-      <c r="I71" s="63">
+      <c r="I71" s="62">
         <v>0</v>
       </c>
-      <c r="J71" s="63" t="s">
+      <c r="J71" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K71" s="64"/>
+      <c r="K71" s="63"/>
     </row>
     <row r="72" customFormat="1" spans="1:11">
       <c r="A72" s="28"/>
@@ -3879,13 +3879,13 @@
         <v>18</v>
       </c>
       <c r="H72" s="44"/>
-      <c r="I72" s="63">
+      <c r="I72" s="62">
         <v>201</v>
       </c>
-      <c r="J72" s="63" t="s">
+      <c r="J72" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="K72" s="64"/>
+      <c r="K72" s="63"/>
     </row>
     <row r="73" customFormat="1" spans="1:11">
       <c r="A73" s="28"/>
@@ -3898,13 +3898,13 @@
         <v>17</v>
       </c>
       <c r="H73" s="44"/>
-      <c r="I73" s="63" t="s">
+      <c r="I73" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J73" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K73" s="64"/>
+      <c r="J73" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K73" s="63"/>
     </row>
     <row r="74" customFormat="1" spans="1:11">
       <c r="A74" s="28"/>
@@ -3923,7 +3923,7 @@
       <c r="J74" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K74" s="64"/>
+      <c r="K74" s="63"/>
     </row>
     <row r="75" customFormat="1" spans="1:11">
       <c r="A75" s="28"/>
@@ -3942,7 +3942,7 @@
       <c r="J75" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K75" s="64"/>
+      <c r="K75" s="63"/>
     </row>
     <row r="76" customFormat="1" ht="14.85" spans="1:11">
       <c r="A76" s="31"/>
@@ -3955,16 +3955,16 @@
         <v>17</v>
       </c>
       <c r="H76" s="54"/>
-      <c r="I76" s="71" t="s">
+      <c r="I76" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J76" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K76" s="72"/>
+      <c r="J76" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="71"/>
     </row>
     <row r="77" customFormat="1" spans="1:11">
-      <c r="A77" s="74" t="s">
+      <c r="A77" s="73" t="s">
         <v>52</v>
       </c>
       <c r="B77" s="34" t="s">
@@ -3978,16 +3978,16 @@
         <v>45</v>
       </c>
       <c r="H77" s="41"/>
-      <c r="I77" s="61"/>
-      <c r="J77" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="K77" s="62" t="s">
+      <c r="I77" s="60"/>
+      <c r="J77" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="K77" s="61" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="78" customFormat="1" spans="1:11">
-      <c r="A78" s="75"/>
+      <c r="A78" s="74"/>
       <c r="B78" s="36"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
@@ -3997,14 +3997,14 @@
         <v>14</v>
       </c>
       <c r="H78" s="44"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="63" t="s">
+      <c r="I78" s="62"/>
+      <c r="J78" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K78" s="64"/>
+      <c r="K78" s="63"/>
     </row>
     <row r="79" customFormat="1" spans="1:11">
-      <c r="A79" s="75"/>
+      <c r="A79" s="74"/>
       <c r="B79" s="36"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
@@ -4014,14 +4014,14 @@
         <v>18</v>
       </c>
       <c r="H79" s="44"/>
-      <c r="I79" s="63"/>
-      <c r="J79" s="63" t="s">
+      <c r="I79" s="62"/>
+      <c r="J79" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K79" s="64"/>
+      <c r="K79" s="63"/>
     </row>
     <row r="80" customFormat="1" spans="1:11">
-      <c r="A80" s="75"/>
+      <c r="A80" s="74"/>
       <c r="B80" s="18"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
@@ -4031,14 +4031,14 @@
         <v>17</v>
       </c>
       <c r="H80" s="44"/>
-      <c r="I80" s="63"/>
-      <c r="J80" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K80" s="64"/>
+      <c r="I80" s="62"/>
+      <c r="J80" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" s="63"/>
     </row>
     <row r="81" customFormat="1" spans="1:11">
-      <c r="A81" s="75"/>
+      <c r="A81" s="74"/>
       <c r="B81" s="30" t="s">
         <v>23</v>
       </c>
@@ -4058,10 +4058,10 @@
       <c r="J81" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K81" s="64"/>
+      <c r="K81" s="63"/>
     </row>
     <row r="82" customFormat="1" spans="1:11">
-      <c r="A82" s="75"/>
+      <c r="A82" s="74"/>
       <c r="B82" s="36"/>
       <c r="C82" s="14"/>
       <c r="D82" s="15"/>
@@ -4079,10 +4079,10 @@
       <c r="J82" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K82" s="64"/>
+      <c r="K82" s="63"/>
     </row>
     <row r="83" customFormat="1" spans="1:11">
-      <c r="A83" s="75"/>
+      <c r="A83" s="74"/>
       <c r="B83" s="36"/>
       <c r="C83" s="14"/>
       <c r="D83" s="15"/>
@@ -4100,10 +4100,10 @@
       <c r="J83" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K83" s="64"/>
+      <c r="K83" s="63"/>
     </row>
     <row r="84" customFormat="1" spans="1:11">
-      <c r="A84" s="75"/>
+      <c r="A84" s="74"/>
       <c r="B84" s="36"/>
       <c r="C84" s="14"/>
       <c r="D84" s="15"/>
@@ -4121,10 +4121,10 @@
       <c r="J84" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K84" s="64"/>
+      <c r="K84" s="63"/>
     </row>
     <row r="85" customFormat="1" ht="14.85" spans="1:11">
-      <c r="A85" s="76"/>
+      <c r="A85" s="75"/>
       <c r="B85" s="37"/>
       <c r="C85" s="23"/>
       <c r="D85" s="24"/>
@@ -4136,13 +4136,13 @@
       <c r="H85" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I85" s="71" t="s">
+      <c r="I85" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J85" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K85" s="72"/>
+      <c r="J85" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K85" s="71"/>
     </row>
     <row r="86" customFormat="1" spans="1:11">
       <c r="A86" s="35" t="s">
@@ -4161,13 +4161,13 @@
       <c r="H86" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="I86" s="61">
+      <c r="I86" s="60">
         <v>414</v>
       </c>
-      <c r="J86" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="K86" s="62" t="s">
+      <c r="J86" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="K86" s="61" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4182,13 +4182,13 @@
         <v>14</v>
       </c>
       <c r="H87" s="44"/>
-      <c r="I87" s="63">
+      <c r="I87" s="62">
         <v>0</v>
       </c>
-      <c r="J87" s="63" t="s">
+      <c r="J87" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K87" s="64"/>
+      <c r="K87" s="63"/>
     </row>
     <row r="88" customFormat="1" spans="1:11">
       <c r="A88" s="28"/>
@@ -4201,13 +4201,13 @@
         <v>18</v>
       </c>
       <c r="H88" s="44"/>
-      <c r="I88" s="63">
-        <v>200</v>
-      </c>
-      <c r="J88" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K88" s="64"/>
+      <c r="I88" s="62">
+        <v>200</v>
+      </c>
+      <c r="J88" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K88" s="63"/>
     </row>
     <row r="89" customFormat="1" spans="1:11">
       <c r="A89" s="28"/>
@@ -4220,13 +4220,13 @@
         <v>17</v>
       </c>
       <c r="H89" s="44"/>
-      <c r="I89" s="63" t="s">
+      <c r="I89" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J89" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K89" s="64"/>
+      <c r="J89" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K89" s="63"/>
     </row>
     <row r="90" customFormat="1" spans="1:11">
       <c r="A90" s="28"/>
@@ -4245,7 +4245,7 @@
       <c r="J90" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K90" s="64"/>
+      <c r="K90" s="63"/>
     </row>
     <row r="91" customFormat="1" spans="1:11">
       <c r="A91" s="28"/>
@@ -4264,7 +4264,7 @@
       <c r="J91" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K91" s="64"/>
+      <c r="K91" s="63"/>
     </row>
     <row r="92" customFormat="1" ht="14.85" spans="1:11">
       <c r="A92" s="31"/>
@@ -4277,13 +4277,13 @@
         <v>17</v>
       </c>
       <c r="H92" s="54"/>
-      <c r="I92" s="71" t="s">
+      <c r="I92" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J92" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K92" s="72"/>
+      <c r="J92" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K92" s="71"/>
     </row>
     <row r="93" customFormat="1" spans="1:11">
       <c r="A93" s="33" t="s">
@@ -4300,13 +4300,13 @@
         <v>14</v>
       </c>
       <c r="H93" s="41"/>
-      <c r="I93" s="61">
+      <c r="I93" s="60">
         <v>0</v>
       </c>
-      <c r="J93" s="61" t="s">
+      <c r="J93" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K93" s="62" t="s">
+      <c r="K93" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4321,32 +4321,32 @@
         <v>18</v>
       </c>
       <c r="H94" s="44"/>
-      <c r="I94" s="63">
+      <c r="I94" s="62">
         <v>201</v>
       </c>
-      <c r="J94" s="63" t="s">
+      <c r="J94" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="K94" s="64"/>
+      <c r="K94" s="63"/>
     </row>
     <row r="95" customFormat="1" ht="14.85" spans="1:11">
       <c r="A95" s="31"/>
       <c r="B95" s="22"/>
-      <c r="C95" s="77"/>
-      <c r="D95" s="78"/>
-      <c r="E95" s="79"/>
-      <c r="F95" s="78"/>
-      <c r="G95" s="80" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="81"/>
-      <c r="I95" s="82" t="s">
+      <c r="C95" s="76"/>
+      <c r="D95" s="77"/>
+      <c r="E95" s="78"/>
+      <c r="F95" s="77"/>
+      <c r="G95" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="80"/>
+      <c r="I95" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="J95" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="K95" s="72"/>
+      <c r="J95" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="K95" s="71"/>
     </row>
     <row r="96" customFormat="1" spans="1:11">
       <c r="A96" s="35" t="s">
@@ -4365,13 +4365,13 @@
       <c r="H96" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="I96" s="73">
+      <c r="I96" s="72">
         <v>413</v>
       </c>
-      <c r="J96" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="K96" s="64" t="s">
+      <c r="J96" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="K96" s="63" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4386,13 +4386,13 @@
         <v>14</v>
       </c>
       <c r="H97" s="44"/>
-      <c r="I97" s="63">
+      <c r="I97" s="62">
         <v>0</v>
       </c>
-      <c r="J97" s="63" t="s">
+      <c r="J97" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K97" s="64"/>
+      <c r="K97" s="63"/>
     </row>
     <row r="98" customFormat="1" spans="1:11">
       <c r="A98" s="28"/>
@@ -4405,13 +4405,13 @@
         <v>18</v>
       </c>
       <c r="H98" s="44"/>
-      <c r="I98" s="63">
-        <v>200</v>
-      </c>
-      <c r="J98" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K98" s="64"/>
+      <c r="I98" s="62">
+        <v>200</v>
+      </c>
+      <c r="J98" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K98" s="63"/>
     </row>
     <row r="99" customFormat="1" spans="1:11">
       <c r="A99" s="28"/>
@@ -4424,13 +4424,13 @@
         <v>17</v>
       </c>
       <c r="H99" s="44"/>
-      <c r="I99" s="63" t="s">
+      <c r="I99" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J99" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K99" s="64"/>
+      <c r="J99" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K99" s="63"/>
     </row>
     <row r="100" customFormat="1" spans="1:11">
       <c r="A100" s="28"/>
@@ -4449,7 +4449,7 @@
       <c r="J100" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K100" s="64"/>
+      <c r="K100" s="63"/>
     </row>
     <row r="101" customFormat="1" spans="1:11">
       <c r="A101" s="28"/>
@@ -4468,7 +4468,7 @@
       <c r="J101" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K101" s="64"/>
+      <c r="K101" s="63"/>
     </row>
     <row r="102" customFormat="1" ht="14.85" spans="1:11">
       <c r="A102" s="31"/>
@@ -4481,13 +4481,13 @@
         <v>17</v>
       </c>
       <c r="H102" s="54"/>
-      <c r="I102" s="71" t="s">
+      <c r="I102" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J102" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K102" s="72"/>
+      <c r="J102" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K102" s="71"/>
     </row>
     <row r="103" customFormat="1" spans="1:11">
       <c r="A103" s="35" t="s">
@@ -4506,13 +4506,13 @@
       <c r="H103" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="I103" s="73">
+      <c r="I103" s="72">
         <v>411</v>
       </c>
-      <c r="J103" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="K103" s="64" t="s">
+      <c r="J103" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="K103" s="63" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4527,13 +4527,13 @@
         <v>14</v>
       </c>
       <c r="H104" s="44"/>
-      <c r="I104" s="63">
+      <c r="I104" s="62">
         <v>0</v>
       </c>
-      <c r="J104" s="63" t="s">
+      <c r="J104" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K104" s="64"/>
+      <c r="K104" s="63"/>
     </row>
     <row r="105" customFormat="1" spans="1:11">
       <c r="A105" s="28"/>
@@ -4546,13 +4546,13 @@
         <v>18</v>
       </c>
       <c r="H105" s="44"/>
-      <c r="I105" s="63">
+      <c r="I105" s="62">
         <v>201</v>
       </c>
-      <c r="J105" s="63" t="s">
+      <c r="J105" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K105" s="64"/>
+      <c r="K105" s="63"/>
     </row>
     <row r="106" customFormat="1" spans="1:11">
       <c r="A106" s="28"/>
@@ -4565,13 +4565,13 @@
         <v>17</v>
       </c>
       <c r="H106" s="44"/>
-      <c r="I106" s="63" t="s">
+      <c r="I106" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J106" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K106" s="64"/>
+      <c r="J106" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K106" s="63"/>
     </row>
     <row r="107" customFormat="1" spans="1:11">
       <c r="A107" s="28"/>
@@ -4590,7 +4590,7 @@
       <c r="J107" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K107" s="64"/>
+      <c r="K107" s="63"/>
     </row>
     <row r="108" customFormat="1" spans="1:11">
       <c r="A108" s="28"/>
@@ -4609,7 +4609,7 @@
       <c r="J108" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K108" s="64"/>
+      <c r="K108" s="63"/>
     </row>
     <row r="109" customFormat="1" ht="14.85" spans="1:11">
       <c r="A109" s="31"/>
@@ -4622,13 +4622,13 @@
         <v>17</v>
       </c>
       <c r="H109" s="54"/>
-      <c r="I109" s="71" t="s">
+      <c r="I109" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J109" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K109" s="72"/>
+      <c r="J109" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K109" s="71"/>
     </row>
     <row r="110" customFormat="1" spans="1:11">
       <c r="A110" s="32" t="s">
@@ -4645,13 +4645,13 @@
         <v>14</v>
       </c>
       <c r="H110" s="41"/>
-      <c r="I110" s="61">
+      <c r="I110" s="60">
         <v>0</v>
       </c>
-      <c r="J110" s="61" t="s">
+      <c r="J110" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K110" s="83" t="s">
+      <c r="K110" s="82" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4666,13 +4666,13 @@
         <v>18</v>
       </c>
       <c r="H111" s="44"/>
-      <c r="I111" s="63">
+      <c r="I111" s="62">
         <v>201</v>
       </c>
-      <c r="J111" s="63" t="s">
+      <c r="J111" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K111" s="64"/>
+      <c r="K111" s="63"/>
     </row>
     <row r="112" customFormat="1" spans="1:11">
       <c r="A112" s="28"/>
@@ -4685,13 +4685,13 @@
         <v>17</v>
       </c>
       <c r="H112" s="44"/>
-      <c r="I112" s="63" t="s">
+      <c r="I112" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J112" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K112" s="64"/>
+      <c r="J112" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K112" s="63"/>
     </row>
     <row r="113" customFormat="1" spans="1:11">
       <c r="A113" s="28"/>
@@ -4712,7 +4712,7 @@
       <c r="J113" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K113" s="64"/>
+      <c r="K113" s="63"/>
     </row>
     <row r="114" customFormat="1" spans="1:11">
       <c r="A114" s="28"/>
@@ -4731,7 +4731,7 @@
       <c r="J114" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K114" s="64"/>
+      <c r="K114" s="63"/>
     </row>
     <row r="115" customFormat="1" ht="14.85" spans="1:11">
       <c r="A115" s="31"/>
@@ -4744,13 +4744,13 @@
         <v>17</v>
       </c>
       <c r="H115" s="54"/>
-      <c r="I115" s="71" t="s">
+      <c r="I115" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J115" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K115" s="72"/>
+      <c r="J115" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K115" s="71"/>
     </row>
     <row r="116" customFormat="1" spans="1:11">
       <c r="A116" s="32" t="s">
@@ -4767,13 +4767,13 @@
         <v>14</v>
       </c>
       <c r="H116" s="41"/>
-      <c r="I116" s="61">
+      <c r="I116" s="60">
         <v>0</v>
       </c>
-      <c r="J116" s="61" t="s">
+      <c r="J116" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K116" s="62" t="s">
+      <c r="K116" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4788,13 +4788,13 @@
         <v>18</v>
       </c>
       <c r="H117" s="44"/>
-      <c r="I117" s="63">
+      <c r="I117" s="62">
         <v>201</v>
       </c>
-      <c r="J117" s="63" t="s">
+      <c r="J117" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K117" s="64"/>
+      <c r="K117" s="63"/>
     </row>
     <row r="118" customFormat="1" spans="1:11">
       <c r="A118" s="28"/>
@@ -4807,13 +4807,13 @@
         <v>17</v>
       </c>
       <c r="H118" s="44"/>
-      <c r="I118" s="63" t="s">
+      <c r="I118" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J118" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K118" s="64"/>
+      <c r="J118" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K118" s="63"/>
     </row>
     <row r="119" customFormat="1" spans="1:11">
       <c r="A119" s="28"/>
@@ -4834,7 +4834,7 @@
       <c r="J119" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K119" s="64"/>
+      <c r="K119" s="63"/>
     </row>
     <row r="120" customFormat="1" spans="1:11">
       <c r="A120" s="28"/>
@@ -4853,7 +4853,7 @@
       <c r="J120" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K120" s="64"/>
+      <c r="K120" s="63"/>
     </row>
     <row r="121" customFormat="1" ht="14.85" spans="1:11">
       <c r="A121" s="31"/>
@@ -4866,13 +4866,13 @@
         <v>17</v>
       </c>
       <c r="H121" s="54"/>
-      <c r="I121" s="71" t="s">
+      <c r="I121" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J121" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K121" s="72"/>
+      <c r="J121" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K121" s="71"/>
     </row>
     <row r="122" customFormat="1" spans="1:11">
       <c r="A122" s="32" t="s">
@@ -4889,13 +4889,13 @@
         <v>14</v>
       </c>
       <c r="H122" s="41"/>
-      <c r="I122" s="61">
+      <c r="I122" s="60">
         <v>0</v>
       </c>
-      <c r="J122" s="61" t="s">
+      <c r="J122" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K122" s="62" t="s">
+      <c r="K122" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4910,13 +4910,13 @@
         <v>18</v>
       </c>
       <c r="H123" s="44"/>
-      <c r="I123" s="63">
-        <v>200</v>
-      </c>
-      <c r="J123" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K123" s="64"/>
+      <c r="I123" s="62">
+        <v>200</v>
+      </c>
+      <c r="J123" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K123" s="63"/>
     </row>
     <row r="124" customFormat="1" ht="14.85" spans="1:11">
       <c r="A124" s="28"/>
@@ -4929,13 +4929,13 @@
         <v>17</v>
       </c>
       <c r="H124" s="44"/>
-      <c r="I124" s="63" t="s">
+      <c r="I124" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J124" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K124" s="64"/>
+      <c r="J124" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K124" s="63"/>
     </row>
     <row r="125" customFormat="1" spans="1:11">
       <c r="A125" s="32" t="s">
@@ -4952,13 +4952,13 @@
         <v>14</v>
       </c>
       <c r="H125" s="41"/>
-      <c r="I125" s="61">
+      <c r="I125" s="60">
         <v>0</v>
       </c>
-      <c r="J125" s="61" t="s">
+      <c r="J125" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K125" s="62" t="s">
+      <c r="K125" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4973,13 +4973,13 @@
         <v>18</v>
       </c>
       <c r="H126" s="44"/>
-      <c r="I126" s="63">
+      <c r="I126" s="62">
         <v>201</v>
       </c>
-      <c r="J126" s="63" t="s">
+      <c r="J126" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K126" s="64"/>
+      <c r="K126" s="63"/>
     </row>
     <row r="127" customFormat="1" spans="1:11">
       <c r="A127" s="28"/>
@@ -4992,13 +4992,13 @@
         <v>17</v>
       </c>
       <c r="H127" s="44"/>
-      <c r="I127" s="63" t="s">
+      <c r="I127" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J127" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K127" s="64"/>
+      <c r="J127" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K127" s="63"/>
     </row>
     <row r="128" customFormat="1" spans="1:11">
       <c r="A128" s="28"/>
@@ -5019,7 +5019,7 @@
       <c r="J128" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K128" s="64"/>
+      <c r="K128" s="63"/>
     </row>
     <row r="129" customFormat="1" spans="1:11">
       <c r="A129" s="28"/>
@@ -5038,7 +5038,7 @@
       <c r="J129" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K129" s="64"/>
+      <c r="K129" s="63"/>
     </row>
     <row r="130" customFormat="1" ht="14.85" spans="1:11">
       <c r="A130" s="31"/>
@@ -5051,13 +5051,13 @@
         <v>17</v>
       </c>
       <c r="H130" s="54"/>
-      <c r="I130" s="71" t="s">
+      <c r="I130" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J130" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K130" s="72"/>
+      <c r="J130" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K130" s="71"/>
     </row>
     <row r="131" customFormat="1" spans="1:11">
       <c r="A131" s="32" t="s">
@@ -5074,13 +5074,13 @@
         <v>14</v>
       </c>
       <c r="H131" s="41"/>
-      <c r="I131" s="61">
+      <c r="I131" s="60">
         <v>0</v>
       </c>
-      <c r="J131" s="61" t="s">
+      <c r="J131" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K131" s="62" t="s">
+      <c r="K131" s="61" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5095,13 +5095,13 @@
         <v>18</v>
       </c>
       <c r="H132" s="44"/>
-      <c r="I132" s="63">
+      <c r="I132" s="62">
         <v>201</v>
       </c>
-      <c r="J132" s="63" t="s">
+      <c r="J132" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="K132" s="64"/>
+      <c r="K132" s="63"/>
     </row>
     <row r="133" customFormat="1" spans="1:11">
       <c r="A133" s="28"/>
@@ -5114,13 +5114,13 @@
         <v>17</v>
       </c>
       <c r="H133" s="44"/>
-      <c r="I133" s="63" t="s">
+      <c r="I133" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="J133" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K133" s="64"/>
+      <c r="J133" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K133" s="63"/>
     </row>
     <row r="134" customFormat="1" spans="1:11">
       <c r="A134" s="28"/>
@@ -5141,7 +5141,7 @@
       <c r="J134" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K134" s="64"/>
+      <c r="K134" s="63"/>
     </row>
     <row r="135" customFormat="1" spans="1:11">
       <c r="A135" s="28"/>
@@ -5160,7 +5160,7 @@
       <c r="J135" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K135" s="64"/>
+      <c r="K135" s="63"/>
     </row>
     <row r="136" customFormat="1" ht="14.85" spans="1:11">
       <c r="A136" s="31"/>
@@ -5173,19 +5173,19 @@
         <v>17</v>
       </c>
       <c r="H136" s="54"/>
-      <c r="I136" s="71" t="s">
+      <c r="I136" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J136" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="K136" s="72"/>
+      <c r="J136" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K136" s="71"/>
     </row>
     <row r="138" spans="1:11">
-      <c r="A138" s="84" t="s">
+      <c r="A138" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="B138" s="84" t="s">
+      <c r="B138" s="83" t="s">
         <v>8</v>
       </c>
       <c r="C138" s="5" t="s">
@@ -5205,10 +5205,10 @@
       <c r="K138" s="5"/>
     </row>
     <row r="139" spans="1:8">
-      <c r="A139" s="85" t="s">
+      <c r="A139" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="B139" s="85" t="s">
+      <c r="B139" s="84" t="s">
         <v>71</v>
       </c>
       <c r="C139" s="3">
@@ -5228,8 +5228,8 @@
       </c>
     </row>
     <row r="140" spans="1:8">
-      <c r="A140" s="85"/>
-      <c r="B140" s="85"/>
+      <c r="A140" s="84"/>
+      <c r="B140" s="84"/>
       <c r="C140" s="3">
         <v>502</v>
       </c>
@@ -5247,8 +5247,8 @@
       </c>
     </row>
     <row r="141" spans="1:8">
-      <c r="A141" s="85"/>
-      <c r="B141" s="85"/>
+      <c r="A141" s="84"/>
+      <c r="B141" s="84"/>
       <c r="C141" s="3">
         <v>503</v>
       </c>
@@ -5265,160 +5265,179 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="85" t="s">
+    <row r="142" spans="1:8">
+      <c r="A142" s="84"/>
+      <c r="B142" s="84"/>
+      <c r="C142" s="3">
+        <v>504</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E142" s="3">
+        <v>454</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B142" s="85" t="s">
+      <c r="B143" s="84" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="85"/>
-      <c r="B143" s="85"/>
-    </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="B144" s="85" t="s">
-        <v>75</v>
-      </c>
+      <c r="A144" s="84"/>
+      <c r="B144" s="84"/>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="85"/>
-      <c r="B145" s="85"/>
+      <c r="A145" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="B145" s="84" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="85" t="s">
+      <c r="A146" s="84"/>
+      <c r="B146" s="84"/>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="B147" s="84" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="84"/>
+      <c r="B148" s="84"/>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B149" s="84" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="84"/>
+      <c r="B150" s="84"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="B151" s="84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="84"/>
+      <c r="B152" s="84"/>
+    </row>
+    <row r="154" spans="1:11">
+      <c r="A154" s="83" t="s">
+        <v>80</v>
+      </c>
+      <c r="B154" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H154" s="5"/>
+      <c r="I154" s="5"/>
+      <c r="J154" s="5"/>
+      <c r="K154" s="5"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="B155" s="84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="84"/>
+      <c r="B156" s="84"/>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="B146" s="85" t="s">
+      <c r="B157" s="84" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="85"/>
-      <c r="B147" s="85"/>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="85" t="s">
+    <row r="158" spans="1:2">
+      <c r="A158" s="84"/>
+      <c r="B158" s="84"/>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="B148" s="85" t="s">
+      <c r="B159" s="84" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="85"/>
-      <c r="B149" s="85"/>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="85" t="s">
+    <row r="160" spans="1:2">
+      <c r="A160" s="84"/>
+      <c r="B160" s="84"/>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="B150" s="85" t="s">
+      <c r="B161" s="84" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="85"/>
-      <c r="B151" s="85"/>
-    </row>
-    <row r="153" spans="1:11">
-      <c r="A153" s="84" t="s">
+    <row r="162" spans="1:2">
+      <c r="A162" s="84"/>
+      <c r="B162" s="84"/>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="B153" s="84" t="s">
-        <v>8</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D153" s="5"/>
-      <c r="E153" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F153" s="5"/>
-      <c r="G153" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H153" s="5"/>
-      <c r="I153" s="5"/>
-      <c r="J153" s="5"/>
-      <c r="K153" s="5"/>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B154" s="85" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="85"/>
-      <c r="B155" s="85"/>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="B156" s="85" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="85"/>
-      <c r="B157" s="85"/>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B158" s="85" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="85"/>
-      <c r="B159" s="85"/>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="B160" s="85" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="85"/>
-      <c r="B161" s="85"/>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="85" t="s">
-        <v>78</v>
-      </c>
-      <c r="B162" s="85" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="85"/>
-      <c r="B163" s="85"/>
-    </row>
-    <row r="165" spans="1:1">
-      <c r="A165" s="84" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166">
+      <c r="B163" s="84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="84"/>
+      <c r="B164" s="84"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167">
         <v>601</v>
       </c>
-      <c r="B166" t="s">
-        <v>81</v>
+      <c r="B167" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -5430,9 +5449,9 @@
     <mergeCell ref="C138:D138"/>
     <mergeCell ref="E138:F138"/>
     <mergeCell ref="G138:K138"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="E153:F153"/>
-    <mergeCell ref="G153:K153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="E154:F154"/>
+    <mergeCell ref="G154:K154"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A19"/>
     <mergeCell ref="A20:A26"/>
@@ -5454,17 +5473,17 @@
     <mergeCell ref="A122:A124"/>
     <mergeCell ref="A125:A130"/>
     <mergeCell ref="A131:A136"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="A139:A142"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="A155:A156"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A159:A160"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A163:A164"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
@@ -5498,17 +5517,17 @@
     <mergeCell ref="B128:B130"/>
     <mergeCell ref="B131:B133"/>
     <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="B158:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B139:B142"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="B155:B156"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B164"/>
     <mergeCell ref="K6:K9"/>
     <mergeCell ref="K10:K13"/>
     <mergeCell ref="K14:K19"/>
@@ -5557,13 +5576,13 @@
   <sheetData>
     <row r="1" ht="14.15" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" ht="14.15" spans="1:3">
@@ -5574,7 +5593,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" ht="14.15" spans="1:3">
@@ -5585,7 +5604,7 @@
         <v>200</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" ht="14.15" spans="1:3">
@@ -5596,7 +5615,7 @@
         <v>200</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" ht="14.15" spans="1:3">
@@ -5607,7 +5626,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" ht="14.15" spans="1:3">
@@ -5618,7 +5637,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" ht="14.15" spans="1:3">
@@ -5629,7 +5648,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" ht="14.15" spans="1:3">
@@ -5640,7 +5659,7 @@
         <v>429</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" ht="14.15" spans="1:3">
@@ -5651,7 +5670,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" ht="14.15" spans="1:3">
@@ -5662,7 +5681,7 @@
         <v>200</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" ht="14.15" spans="1:3">
@@ -5673,7 +5692,7 @@
         <v>200</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" ht="14.15" spans="1:3">
@@ -5684,7 +5703,7 @@
         <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" ht="14.15" spans="1:3">
@@ -5695,7 +5714,7 @@
         <v>200</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" ht="14.15" spans="1:3">
@@ -5706,7 +5725,7 @@
         <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" ht="14.15" spans="1:3">
@@ -5717,7 +5736,7 @@
         <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" ht="14.15" spans="1:3">
@@ -5728,7 +5747,7 @@
         <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" ht="14.15" spans="1:3">
@@ -5739,7 +5758,7 @@
         <v>200</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" ht="14.15" spans="1:3">
@@ -5750,7 +5769,7 @@
         <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" ht="14.15" spans="1:3">
@@ -5761,7 +5780,7 @@
         <v>200</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" ht="14.15" spans="1:3">
@@ -5772,7 +5791,7 @@
         <v>200</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" ht="14.15" spans="1:3">
@@ -5783,7 +5802,7 @@
         <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" ht="14.15" spans="1:3">
@@ -5794,7 +5813,7 @@
         <v>200</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" ht="14.15" spans="1:3">
@@ -5805,7 +5824,7 @@
         <v>200</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" ht="14.15" spans="1:3">
@@ -5816,7 +5835,7 @@
         <v>200</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" ht="14.15" spans="1:3">
@@ -5827,7 +5846,7 @@
         <v>200</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" ht="14.15" spans="1:3">
@@ -5838,7 +5857,7 @@
         <v>200</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" ht="14.15" spans="1:3">
@@ -5849,7 +5868,7 @@
         <v>200</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" ht="14.15" spans="1:3">
@@ -5860,7 +5879,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" ht="14.15" spans="1:3">
@@ -5871,7 +5890,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" ht="14.15" spans="1:3">
@@ -5882,7 +5901,7 @@
         <v>200</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" ht="14.15" spans="1:3">
@@ -5893,7 +5912,7 @@
         <v>200</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" ht="14.15" spans="1:3">
@@ -5904,7 +5923,7 @@
         <v>200</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" ht="14.15" spans="1:3">
@@ -5915,7 +5934,7 @@
         <v>200</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" ht="14.15" spans="1:3">
@@ -5926,7 +5945,7 @@
         <v>200</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" ht="14.15" spans="1:3">
@@ -5937,7 +5956,7 @@
         <v>200</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" ht="14.15" spans="1:3">
@@ -5948,7 +5967,7 @@
         <v>200</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" ht="14.15" spans="1:3">
@@ -5959,7 +5978,7 @@
         <v>200</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" ht="14.15" spans="1:3">
@@ -5970,7 +5989,7 @@
         <v>200</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" ht="14.15" spans="1:3">
@@ -5981,7 +6000,7 @@
         <v>200</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" ht="14.15" spans="1:3">
@@ -5992,7 +6011,7 @@
         <v>200</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" ht="14.15" spans="1:3">
@@ -6003,7 +6022,7 @@
         <v>200</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" ht="14.15" spans="1:3">
@@ -6014,7 +6033,7 @@
         <v>200</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" ht="14.15" spans="1:3">
@@ -6025,7 +6044,7 @@
         <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" ht="14.15" spans="1:3">
@@ -6036,7 +6055,7 @@
         <v>200</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" ht="14.15" spans="1:3">
@@ -6047,7 +6066,7 @@
         <v>200</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" ht="14.15" spans="1:3">
@@ -6058,7 +6077,7 @@
         <v>200</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" ht="14.15" spans="1:3">
@@ -6069,7 +6088,7 @@
         <v>200</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" ht="14.15" spans="1:3">
@@ -6080,7 +6099,7 @@
         <v>200</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" ht="14.15" spans="1:3">
@@ -6091,7 +6110,7 @@
         <v>200</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" ht="14.15" spans="1:3">
@@ -6102,7 +6121,7 @@
         <v>200</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" ht="14.15" spans="1:3">
@@ -6113,7 +6132,7 @@
         <v>200</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" ht="14.15" spans="1:3">
@@ -6124,7 +6143,7 @@
         <v>200</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" ht="14.15" spans="1:3">
@@ -6135,7 +6154,7 @@
         <v>200</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" ht="14.15" spans="1:3">
@@ -6146,7 +6165,7 @@
         <v>200</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" ht="14.15" spans="1:3">
@@ -6157,7 +6176,7 @@
         <v>200</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" ht="14.15" spans="1:3">
@@ -6168,7 +6187,7 @@
         <v>200</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" ht="14.15" spans="1:3">
@@ -6179,7 +6198,7 @@
         <v>200</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" ht="14.15" spans="1:3">
@@ -6190,7 +6209,7 @@
         <v>200</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" ht="14.15" spans="1:3">
@@ -6201,7 +6220,7 @@
         <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" ht="14.15" spans="1:3">
@@ -6212,7 +6231,7 @@
         <v>200</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" ht="14.15" spans="1:3">
@@ -6223,7 +6242,7 @@
         <v>200</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" ht="14.15" spans="1:3">
@@ -6234,7 +6253,7 @@
         <v>200</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" ht="14.15" spans="1:3">
@@ -6245,7 +6264,7 @@
         <v>200</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" ht="14.15" spans="1:3">
@@ -6256,7 +6275,7 @@
         <v>200</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" ht="14.15" spans="1:3">
@@ -6267,7 +6286,7 @@
         <v>200</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major Savepoint; FCRT 2.1.3 finished, 100%; API/WSS Request Flow updated; contexts and sources added to standardized message object for reporting; next up: FCRT 2.1.4;
</commit_message>
<xml_diff>
--- a/~Documents/api-error.xlsx
+++ b/~Documents/api-error.xlsx
@@ -479,9 +479,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -523,8 +523,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -533,9 +556,32 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -549,22 +595,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,21 +603,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,7 +624,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -624,7 +646,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -632,31 +654,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -681,7 +681,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,7 +771,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,103 +831,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,49 +855,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1569,17 +1569,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1602,21 +1602,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1628,6 +1613,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1671,82 +1671,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="62" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="62" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="61" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1755,64 +1755,64 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="59" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="59" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="59" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2393,8 +2393,8 @@
   <sheetPr/>
   <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="T137" sqref="T137:T138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1"/>

</xml_diff>

<commit_message>
Savepoint; Interim code WIP; DDL changes for refactored stops handling; stops are loading history with nominal issues incl. initial request status; fix: if history and stop is 'live' or 'effective', set to 'Expired'; issue brought up Blofin - no fix planned; Blofin TPSL data architecture is 1NF where our DA (pertaining to stops) is 2NF/3NF hybrid providing atomic control by stop type (seperation of orders); due to the first normal form repeating group of the Blofin API DDL re: TPSL, the hybrid approach is the most performant and is integrated as is. Next up: refactors: TPSL cancels, queue processing and submit functionality; then FCRT 2.2.1-4 completion;
</commit_message>
<xml_diff>
--- a/~Documents/api-error.xlsx
+++ b/~Documents/api-error.xlsx
@@ -4,18 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15638"/>
+    <workbookView windowHeight="15638" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="baseline">[1]stop_request!$A$3:$A$22</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="151">
   <si>
     <t>Outcome Matrix</t>
   </si>
@@ -269,7 +275,10 @@
     <t>System Level Errors:</t>
   </si>
   <si>
-    <t>Critical System Error: Required states (Expired/Hold) are missing from cache</t>
+    <t>System Configuration: Required states (Expired/Hold) are missing from cache</t>
+  </si>
+  <si>
+    <t>System Configuration: Required stop types (tp/sl) are missing from cache</t>
   </si>
   <si>
     <t>error_code</t>
@@ -478,10 +487,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -531,13 +540,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -546,17 +548,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,61 +602,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -638,18 +622,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -681,19 +690,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,31 +786,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,31 +846,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,85 +858,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1584,20 +1593,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1617,17 +1623,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1646,167 +1675,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="61" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="62" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="56" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="57" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="57" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="62" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="61" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="60" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="59" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="58" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="59" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2131,6 +2140,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Summary"/>
+      <sheetName val="stop_request"/>
+      <sheetName val="stop_order"/>
+      <sheetName val="vw_stop_orders"/>
+      <sheetName val="vw_api_stop_requests"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2391,10 +2421,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M167"/>
+  <dimension ref="A1:M168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="T137" sqref="T137:T138"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="H171" sqref="H171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1"/>
@@ -5438,6 +5468,14 @@
       </c>
       <c r="B167" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168">
+        <v>602</v>
+      </c>
+      <c r="B168" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -5562,8 +5600,8 @@
   <sheetPr/>
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="102.377777777778" defaultRowHeight="14.1" outlineLevelCol="2"/>
@@ -5576,13 +5614,13 @@
   <sheetData>
     <row r="1" ht="14.15" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" ht="14.15" spans="1:3">
@@ -5593,7 +5631,7 @@
         <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" ht="14.15" spans="1:3">
@@ -5604,7 +5642,7 @@
         <v>200</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" ht="14.15" spans="1:3">
@@ -5615,7 +5653,7 @@
         <v>200</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" ht="14.15" spans="1:3">
@@ -5626,7 +5664,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="14.15" spans="1:3">
@@ -5637,7 +5675,7 @@
         <v>200</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" ht="14.15" spans="1:3">
@@ -5648,7 +5686,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" ht="14.15" spans="1:3">
@@ -5659,7 +5697,7 @@
         <v>429</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" ht="14.15" spans="1:3">
@@ -5670,7 +5708,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" ht="14.15" spans="1:3">
@@ -5681,7 +5719,7 @@
         <v>200</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" ht="14.15" spans="1:3">
@@ -5692,7 +5730,7 @@
         <v>200</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" ht="14.15" spans="1:3">
@@ -5703,7 +5741,7 @@
         <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" ht="14.15" spans="1:3">
@@ -5714,7 +5752,7 @@
         <v>200</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="14.15" spans="1:3">
@@ -5725,7 +5763,7 @@
         <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" ht="14.15" spans="1:3">
@@ -5736,7 +5774,7 @@
         <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" ht="14.15" spans="1:3">
@@ -5747,7 +5785,7 @@
         <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" ht="14.15" spans="1:3">
@@ -5758,7 +5796,7 @@
         <v>200</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" ht="14.15" spans="1:3">
@@ -5769,7 +5807,7 @@
         <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" ht="14.15" spans="1:3">
@@ -5780,7 +5818,7 @@
         <v>200</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" ht="14.15" spans="1:3">
@@ -5791,7 +5829,7 @@
         <v>200</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" ht="14.15" spans="1:3">
@@ -5802,7 +5840,7 @@
         <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" ht="14.15" spans="1:3">
@@ -5813,7 +5851,7 @@
         <v>200</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" ht="14.15" spans="1:3">
@@ -5824,7 +5862,7 @@
         <v>200</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" ht="14.15" spans="1:3">
@@ -5835,7 +5873,7 @@
         <v>200</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" ht="14.15" spans="1:3">
@@ -5846,7 +5884,7 @@
         <v>200</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" ht="14.15" spans="1:3">
@@ -5857,7 +5895,7 @@
         <v>200</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" ht="14.15" spans="1:3">
@@ -5868,7 +5906,7 @@
         <v>200</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" ht="14.15" spans="1:3">
@@ -5879,7 +5917,7 @@
         <v>200</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" ht="14.15" spans="1:3">
@@ -5890,7 +5928,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" ht="14.15" spans="1:3">
@@ -5901,7 +5939,7 @@
         <v>200</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" ht="14.15" spans="1:3">
@@ -5912,7 +5950,7 @@
         <v>200</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" ht="14.15" spans="1:3">
@@ -5923,7 +5961,7 @@
         <v>200</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" ht="14.15" spans="1:3">
@@ -5934,7 +5972,7 @@
         <v>200</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" ht="14.15" spans="1:3">
@@ -5945,7 +5983,7 @@
         <v>200</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" ht="14.15" spans="1:3">
@@ -5956,7 +5994,7 @@
         <v>200</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" ht="14.15" spans="1:3">
@@ -5967,7 +6005,7 @@
         <v>200</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" ht="14.15" spans="1:3">
@@ -5978,7 +6016,7 @@
         <v>200</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" ht="14.15" spans="1:3">
@@ -5989,7 +6027,7 @@
         <v>200</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" ht="14.15" spans="1:3">
@@ -6000,7 +6038,7 @@
         <v>200</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" ht="14.15" spans="1:3">
@@ -6011,7 +6049,7 @@
         <v>200</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" ht="14.15" spans="1:3">
@@ -6022,7 +6060,7 @@
         <v>200</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" ht="14.15" spans="1:3">
@@ -6033,7 +6071,7 @@
         <v>200</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" ht="14.15" spans="1:3">
@@ -6044,7 +6082,7 @@
         <v>200</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" ht="14.15" spans="1:3">
@@ -6055,7 +6093,7 @@
         <v>200</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" ht="14.15" spans="1:3">
@@ -6066,7 +6104,7 @@
         <v>200</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" ht="14.15" spans="1:3">
@@ -6077,7 +6115,7 @@
         <v>200</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" ht="14.15" spans="1:3">
@@ -6088,7 +6126,7 @@
         <v>200</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" ht="14.15" spans="1:3">
@@ -6099,7 +6137,7 @@
         <v>200</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" ht="14.15" spans="1:3">
@@ -6110,7 +6148,7 @@
         <v>200</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" ht="14.15" spans="1:3">
@@ -6121,7 +6159,7 @@
         <v>200</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" ht="14.15" spans="1:3">
@@ -6132,7 +6170,7 @@
         <v>200</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" ht="14.15" spans="1:3">
@@ -6143,7 +6181,7 @@
         <v>200</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" ht="14.15" spans="1:3">
@@ -6154,7 +6192,7 @@
         <v>200</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" ht="14.15" spans="1:3">
@@ -6165,7 +6203,7 @@
         <v>200</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" ht="14.15" spans="1:3">
@@ -6176,7 +6214,7 @@
         <v>200</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" ht="14.15" spans="1:3">
@@ -6187,7 +6225,7 @@
         <v>200</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" ht="14.15" spans="1:3">
@@ -6198,7 +6236,7 @@
         <v>200</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" ht="14.15" spans="1:3">
@@ -6209,7 +6247,7 @@
         <v>200</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" ht="14.15" spans="1:3">
@@ -6220,7 +6258,7 @@
         <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" ht="14.15" spans="1:3">
@@ -6231,7 +6269,7 @@
         <v>200</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" ht="14.15" spans="1:3">
@@ -6242,7 +6280,7 @@
         <v>200</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" ht="14.15" spans="1:3">
@@ -6253,7 +6291,7 @@
         <v>200</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" ht="14.15" spans="1:3">
@@ -6264,7 +6302,7 @@
         <v>200</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" ht="14.15" spans="1:3">
@@ -6275,7 +6313,7 @@
         <v>200</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" ht="14.15" spans="1:3">
@@ -6286,7 +6324,7 @@
         <v>200</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>